<commit_message>
se agregaron los indicadores y conclusiones de solapa de vivienda y suelo
</commit_message>
<xml_diff>
--- a/data/santa-maria-conclusiones.xlsx
+++ b/data/santa-maria-conclusiones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="127">
   <si>
     <t xml:space="preserve">ESCALA</t>
   </si>
@@ -103,6 +103,36 @@
     <t xml:space="preserve">Andalhualá</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 54 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda sin hacinamiento en el área de estudio alcanza niveles de acceso generalizados, ya que más del 80% de los hogares no se encuentran en situación de hacinamiento. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de programa de generación de lotes con servicios. El accionar estatal a través de normas y programas muestra que hay existencia de legislación que consagra el derecho a una vivienda adecuada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de políticas de Alquiler Social o regulaciones específicas; y no hay existencia de Código de Edificación actualizado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 74 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las viviendas con baño propio en el área de estudio alcanzan niveles de acceso generalizados, ya que más del 80% de los hogares residen en viviendas que tienen. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de módulos sanitarios; no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción; no hay existencia de programas de mejoramiento de viviendas; y no hay existencia de planes de urbanización en áreas vulnerables. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda adecuada en el área de estudio alcanza niveles de acceso generalizados, ya que más del 80% de los hogares habitan en viviendas que no son de tipo inconveniente. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que hay existencia de legislación que consagra el derecho a una vivienda adecuada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; y no hay existencia de políticas de Alquiler Social o regulaciones específicas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la provisión de agua potable en el área de estudio alcanza niveles de acceso generalizados, ya que más del 80% de los hogares acceden al mismo. Este valor se explica principalmente por la obra pública, con una cobertura que abarca casi a la totalidad de las conexiones. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al agua potable; hay presencia de Plan Maestro, Director o Estratégico de agua actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de agua; y no hay presencia de estructura tarifaria regulada o programas de subsidios tarifarios para el agua.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 59 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Según el análisis de los datos provistos por el registro DESINVENTAR, no hay presencia de amenazas biológicas; no hay presencia de amenazas físico químicas; no hay presencia de amenazas geodinámicas; y hay presencia de amenazas hidrometeorológicas.El accionar estatal a través de normas y programas muestra que hay presencia de Marco Legal de Gestión Integral del Riesgo de Desastres (GIRD); no hay presencia de normas municipales de regulación de uso del suelo y edificación que mitigen riesgos; hay presencia de sistemas oficiales de Alerta Temprana; y no hay presencia de fondos específicos para Mitigación de Riesgos de Desastres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la energía en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden a la misma. Este valor da cuenta que menos de la mitad de los hogares cocinan con gas en tubo o a granel (zeppelin) o gas en garrafa. El accionar estatal a través de normas y programas muestra que no hay presencia de una estructura tarifaria regulada o programas de subsidios tarifarios para el servicio de energia o gas en la jurisdicción; no hay presencia de un Plan de obras o similar actualizado; hay presencia de un ente regulador formal (provincial/municipal) para el servicio de electricidad o gas; y no hay presencia de normativas provinciales o municipales que regulen la seguridad de las instalaciones eléctricas y/o de gas domiciliarias. Es importante destacar que el 42 % de los hogares no accede al cumplimiento del derecho a energía segura ya que utilizan leña, carbón i otro combustible para cocinar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a las telecomunicaciones en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden al mismo. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de Servicio Básico Universal (SBU) o Tarifa Social para internet y/o telefonía móvil en la jurisdicción; no hay existencia de normativas provinciales o municipales que faciliten el despliegue de infraestructura de telecomunicaciones (ej. antenas, fibra óptica); hay existencia de un ente regulador formal (provincial/municipal) para el servicio de telecomunicaciones; y no hay existencia de espacios públicos que permitan el libre acceso a internet. Es importante destacar que el 58 % de los hogares no tiene acceso a telecomunicaciones.</t>
+  </si>
+  <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
@@ -118,24 +148,15 @@
     <t xml:space="preserve">E</t>
   </si>
   <si>
-    <t xml:space="preserve">El cumplimiento del derecho a la provisión de agua potable en el área de estudio alcanza niveles de acceso generalizados, ya que más del 80% de los hogares acceden al mismo. Este valor se explica principalmente por la obra pública, con una cobertura que abarca casi a la totalidad de las conexiones. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al agua potable; hay presencia de Plan Maestro, Director o Estratégico de agua actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de agua; y no hay presencia de estructura tarifaria regulada o programas de subsidios tarifarios para el agua.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 59 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Según el análisis de los datos provistos por el registro DESINVENTAR, no hay presencia de amenazas biológicas; no hay presencia de amenazas físico químicas; no hay presencia de amenazas geodinámicas; y hay presencia de amenazas hidrometeorológicas.El accionar estatal a través de normas y programas muestra que hay presencia de Marco Legal de Gestión Integral del Riesgo de Desastres (GIRD); no hay presencia de normas municipales de regulación de uso del suelo y edificación que mitigen riesgos; hay presencia de sistemas oficiales de Alerta Temprana; y no hay presencia de fondos específicos para Mitigación de Riesgos de Desastres.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El cumplimiento del derecho a la energía en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden a la misma. Este valor da cuenta que menos de la mitad de los hogares cocinan con gas en tubo o a granel (zeppelin) o gas en garrafa. El accionar estatal a través de normas y programas muestra que no hay presencia de una estructura tarifaria regulada o programas de subsidios tarifarios para el servicio de energia o gas en la jurisdicción; no hay presencia de un Plan de obras o similar actualizado; hay presencia de un ente regulador formal (provincial/municipal) para el servicio de electricidad o gas; y no hay presencia de normativas provinciales o municipales que regulen la seguridad de las instalaciones eléctricas y/o de gas domiciliarias. Es importante destacar que el 42 % de los hogares no accede al cumplimiento del derecho a energía segura ya que utilizan leña, carbón i otro combustible para cocinar.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El cumplimiento del derecho a las telecomunicaciones en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden al mismo. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de Servicio Básico Universal (SBU) o Tarifa Social para internet y/o telefonía móvil en la jurisdicción; no hay existencia de normativas provinciales o municipales que faciliten el despliegue de infraestructura de telecomunicaciones (ej. antenas, fibra óptica); hay existencia de un ente regulador formal (provincial/municipal) para el servicio de telecomunicaciones; y no hay existencia de espacios públicos que permitan el libre acceso a internet. Es importante destacar que el 58 % de los hogares no tiene acceso a telecomunicaciones.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chañar Punco</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 60 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 46 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 36 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
   </si>
   <si>
@@ -148,6 +169,12 @@
     <t xml:space="preserve">Departamento de Santa María</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 48 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 32 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares acceden al mismo. Este valor se explica por una relación equitativa de esfuerzos tanto del sector público a través de la obra pública y la organización social. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 22 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
   </si>
   <si>
@@ -157,6 +184,12 @@
     <t xml:space="preserve">El Cajón</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 71 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio es muy limitado, donde menos del 20% de los hogares se encuentran construidas con materiales adecuados, indicando una situación crítica de alta vulnerabilidad. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 95 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho a la provisión de agua potable en el área de estudio es muy limitado, donde menos del 20% de los hogares tienen acceso, indicando una situación crítica de alta vulnerabilidad. Este valor se explica por la falta, tanto de obra pública como de iniciativa privada, lo que resulta en una cobertura insuficiente para garantizar el derecho. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al agua potable; hay presencia de Plan Maestro, Director o Estratégico de agua actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de agua; y no hay presencia de estructura tarifaria regulada o programas de subsidios tarifarios para el agua. Es importante destacar que el 84 % de los hogares no accede al cumplimiento del derecho a agua segura ya que utiliza agua proveniente de pozo sin bomba, transporte por cisterna, agua de lluvia, río, canal, arroyo o acequia u otra procedencia para cocinar.</t>
   </si>
   <si>
@@ -172,6 +205,12 @@
     <t xml:space="preserve">El Desmonte</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 73 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 68 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho a la provisión de agua potable en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares acceden al mismo. Este valor se explica principalmente por la obra pública, con una cobertura donde la red pública garantiza 3 de cada 4 conexiones en los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al agua potable; hay presencia de Plan Maestro, Director o Estratégico de agua actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de agua; y no hay presencia de estructura tarifaria regulada o programas de subsidios tarifarios para el agua. Es importante destacar que el 25 % de los hogares no accede al cumplimiento del derecho a agua segura ya que utiliza agua proveniente de pozo sin bomba, transporte por cisterna, agua de lluvia, río, canal, arroyo o acequia u otra procedencia para cocinar.</t>
   </si>
   <si>
@@ -187,6 +226,9 @@
     <t xml:space="preserve">El Puesto</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 61 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 50 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
   </si>
   <si>
@@ -196,6 +238,12 @@
     <t xml:space="preserve">Famatanca</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 70 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 51 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 43 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
   </si>
   <si>
@@ -205,12 +253,27 @@
     <t xml:space="preserve">Fuerte Quemado</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 62 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 44 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 28 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
   </si>
   <si>
     <t xml:space="preserve">La Hoyada</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 34 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio es muy limitado, donde menos del 20% de los hogares se encuentran construidas con materiales adecuados, indicando una situación crítica de alta vulnerabilidad. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 85 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las viviendas con baño propio en el área de estudio alcanzan niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares residen en viviendas que tienen. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de módulos sanitarios; no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción; no hay existencia de programas de mejoramiento de viviendas; y no hay existencia de planes de urbanización en áreas vulnerables. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 34 % de los hogares no residen en viviendas con baños propios.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho a la provisión de agua potable en el área de estudio es muy limitado, donde menos del 20% de los hogares tienen acceso, indicando una situación crítica de alta vulnerabilidad. Este valor se explica por la falta, tanto de obra pública como de iniciativa privada, lo que resulta en una cobertura insuficiente para garantizar el derecho. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al agua potable; hay presencia de Plan Maestro, Director o Estratégico de agua actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de agua; y no hay presencia de estructura tarifaria regulada o programas de subsidios tarifarios para el agua. Es importante destacar que el 83 % de los hogares no accede al cumplimiento del derecho a agua segura ya que utiliza agua proveniente de pozo sin bomba, transporte por cisterna, agua de lluvia, río, canal, arroyo o acequia u otra procedencia para cocinar.</t>
   </si>
   <si>
@@ -223,6 +286,12 @@
     <t xml:space="preserve">Las Mojarras</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 57 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 41 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 27 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
   </si>
   <si>
@@ -232,6 +301,9 @@
     <t xml:space="preserve">Municipio de San José</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 53 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 38 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
   </si>
   <si>
@@ -241,6 +313,12 @@
     <t xml:space="preserve">Municipio de Santa María</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 43 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 24 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso generalizados, ya que más del 80% de los hogares acceden al mismo. Este valor se explica principalmente por la obra pública, con una cobertura donde la red pública garantiza al menos la mitad de las conexiones en los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido.</t>
   </si>
   <si>
@@ -250,6 +328,12 @@
     <t xml:space="preserve">Punta de Balasto</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio es muy limitado, donde menos del 20% de los hogares son propietarios o alquilan, indicando una situación crítica de alta vulnerabilidad. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 81 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 26 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 54 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
   </si>
   <si>
@@ -259,12 +343,24 @@
     <t xml:space="preserve">San José</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 56 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 42 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho a las telecomunicaciones en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares acceden al mismo. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de Servicio Básico Universal (SBU) o Tarifa Social para internet y/o telefonía móvil en la jurisdicción; no hay existencia de normativas provinciales o municipales que faciliten el despliegue de infraestructura de telecomunicaciones (ej. antenas, fibra óptica); hay existencia de un ente regulador formal (provincial/municipal) para el servicio de telecomunicaciones; y no hay existencia de espacios públicos que permitan el libre acceso a internet. Es importante destacar que el 33 % de los hogares no tiene acceso a telecomunicaciones.</t>
   </si>
   <si>
     <t xml:space="preserve">Santa María</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 44 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio alcanza niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares se encuentran construidas con materiales adecuados. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso generalizados, ya que más del 80% de los hogares acceden al mismo. Este valor se explica principalmente por la obra pública, con una cobertura donde la red pública garantiza 3 de cada 4 conexiones en los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido.</t>
   </si>
   <si>
@@ -274,6 +370,9 @@
     <t xml:space="preserve">Yapes</t>
   </si>
   <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 74 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El cumplimiento del derecho a la provisión de agua potable en el área de estudio alcanza niveles de acceso limitados, ya que entre el 40% y el 60% los hogares acceden al mismo. Este valor se explica principalmente por la obra pública, con una cobertura donde la red pública garantiza al menos la mitad de las conexiones en los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al agua potable; hay presencia de Plan Maestro, Director o Estratégico de agua actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de agua; y no hay presencia de estructura tarifaria regulada o programas de subsidios tarifarios para el agua. Es importante destacar que el 44 % de los hogares no accede al cumplimiento del derecho a agua segura ya que utiliza agua proveniente de pozo sin bomba, transporte por cisterna, agua de lluvia, río, canal, arroyo o acequia u otra procedencia para cocinar.</t>
   </si>
   <si>
@@ -284,6 +383,15 @@
   </si>
   <si>
     <t xml:space="preserve">Zona Rural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a la seguridad en la tenencia en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares son propietarios o alquilan. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de hogares que hayan sido beneficiados por proyectos de integración socio-urbana; no hay existencia de planes de urbanización en áreas vulnerables; no hay existencia de obras de infraestructura en sectores degradados; y no hay existencia de obras de mejora de viviendas. El accionar estatal a través de normas y programas muestra que hay existencia de leyes y políticas públicas reconocen y protegen diversas formas de tenencia (propiedad, usufructo, posesión, alquiler, tenencia comunitaria, etc.; no hay existencia de sistemas catastrales y registrales actualizados, eficientes y accesibles que permitan inscribir los derechos de tenencia; no hay existencia de marco normativo de protección contra Desalojos Forzosos; y no hay existencia de normas o programas locales específicos de regularización dominial. Es importante destacar que el 64 % de los hogares no tiene garantizada una tenencia segura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cumplimiento del derecho a una vivienda construida con materiales adecuados en el área de estudio es muy limitado, donde menos del 20% de los hogares se encuentran construidas con materiales adecuados, indicando una situación crítica de alta vulnerabilidad. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de viviendas sociales; no hay existencia de programas de mejoramiento de viviendas; no hay existencia de planes de urbanización en áreas vulnerables; y no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 93 % de los hogares no se encuentran construidas con materiales adecuados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las viviendas con baño propio en el área de estudio alcanzan niveles de acceso adecuados, ya que entre el 60% y el 80% los hogares residen en viviendas que tienen. El estudio del alcance de las obras públicas dan cuenta que no hay existencia de programas de construcción de módulos sanitarios; no hay existencia de provisión de materiales o Asistencia Técnica para la autoconstrucción; no hay existencia de programas de mejoramiento de viviendas; y no hay existencia de planes de urbanización en áreas vulnerables. El accionar estatal a través de normas y programas muestra que no hay existencia de programas de apoyo a Cooperativas de Vivienda o Construcción Autogestionada; no hay existencia de créditos accesibles o subsidios para la construcción y/o mejora habitacional; no hay existencia de instrumentos de Fiscalización y Habilitación de Obras; y no hay existencia de Código de Edificación actualizado. Es importante destacar que el 21 % de los hogares no residen en viviendas con baños propios.</t>
   </si>
   <si>
     <t xml:space="preserve">El cumplimiento del derecho al saneamiento en el área de estudio alcanza niveles de acceso deficiente, ya que menos del 40% los hogares acceden al mismo. Este valor se alcanza gracias al esfuerzo privado, que descargan a cámara séptica y pozo ciego individual, donde las obras privadas no alcanzan a la mitad de los hogares. El accionar estatal a través de normas y programas muestra que hay presencia de legislación que consagra el derecho al saneamiento adecuado; no hay presencia de Plan Maestro, Director o Estratégico de saneamiento actualizado; hay presencia de Ente regulador formal (provincial/municipal) para el servicio de saneamiento; y no hay presencia de normativas provinciales o municipales que regulen la descarga de efluentes cloacales y/o exijan su tratamiento antes del vertido. Es importante destacar que el 75 % de los hogares no descarga a saneamiento seguro ya que lo hace sólo pozo ciego o a hoyo, excavación en la tierra, etc.</t>
@@ -382,7 +490,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -393,6 +501,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -593,8 +705,8 @@
   </sheetPr>
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z21" activeCellId="0" sqref="Z21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -691,19 +803,19 @@
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -722,49 +834,49 @@
         <v>36</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,82 +884,82 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,82 +967,82 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,82 +1050,82 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,82 +1133,82 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,82 +1216,82 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,82 +1299,82 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,82 +1382,82 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,25 +1465,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="E10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>33</v>
@@ -1380,55 +1492,55 @@
         <v>34</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,82 +1548,82 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,82 +1631,82 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,82 +1714,82 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,82 +1797,82 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,82 +1880,82 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,82 +1963,82 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,82 +2046,82 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2017,86 +2129,86 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="E18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M23" s="3"/>
+      <c r="M23" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>